<commit_message>
Some cases added for test suite. Attempts to unify the point cloud reader and body builder stuff again.
</commit_message>
<xml_diff>
--- a/LUMA/cases/TestSuiteIndex.xlsx
+++ b/LUMA/cases/TestSuiteIndex.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="65">
   <si>
     <t>Case #</t>
   </si>
@@ -200,6 +200,27 @@
   </si>
   <si>
     <t>3 Grid + 3D + MPI</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Umax</t>
+  </si>
+  <si>
+    <t>1.5 * Uref</t>
+  </si>
+  <si>
+    <t>NumMarkers</t>
+  </si>
+  <si>
+    <t>gravity force</t>
   </si>
 </sst>
 </file>
@@ -632,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:W73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,19 +671,20 @@
     <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -693,41 +715,44 @@
       <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
@@ -740,23 +765,24 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="6"/>
+      <c r="Q2" s="7"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="6"/>
+      <c r="V2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -788,40 +814,43 @@
         <v>16</v>
       </c>
       <c r="K3" s="1">
+        <v>120</v>
+      </c>
+      <c r="L3" s="1">
         <v>0</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -853,40 +882,43 @@
         <v>16</v>
       </c>
       <c r="K4" s="1">
+        <v>120</v>
+      </c>
+      <c r="L4" s="1">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -918,13 +950,13 @@
         <v>16</v>
       </c>
       <c r="K5" s="1">
+        <v>120</v>
+      </c>
+      <c r="L5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>28</v>
@@ -933,25 +965,28 @@
         <v>28</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -982,41 +1017,44 @@
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="V6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1047,14 +1085,14 @@
       <c r="J7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>28</v>
@@ -1063,25 +1101,28 @@
         <v>28</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="V7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1112,41 +1153,44 @@
       <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M8" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="V8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>47</v>
       </c>
@@ -1167,8 +1211,15 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T9" s="1"/>
+      <c r="V9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="W9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1199,35 +1250,44 @@
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1">
         <v>0</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1258,14 +1318,14 @@
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>28</v>
@@ -1274,19 +1334,28 @@
         <v>28</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="W11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1317,35 +1386,44 @@
       <c r="J12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1">
         <v>0</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M12" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1376,35 +1454,44 @@
       <c r="J13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1">
         <v>0</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W13">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>48</v>
       </c>
@@ -1425,8 +1512,9 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1458,34 +1546,37 @@
         <v>16</v>
       </c>
       <c r="K15" s="1">
+        <v>120</v>
+      </c>
+      <c r="L15" s="1">
         <v>1</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P15" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1517,34 +1608,37 @@
         <v>16</v>
       </c>
       <c r="K16" s="1">
+        <v>120</v>
+      </c>
+      <c r="L16" s="1">
         <v>1</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P16" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1576,13 +1670,13 @@
         <v>16</v>
       </c>
       <c r="K17" s="1">
+        <v>120</v>
+      </c>
+      <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M17" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>28</v>
@@ -1591,19 +1685,22 @@
         <v>28</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1634,35 +1731,38 @@
       <c r="J18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1693,14 +1793,14 @@
       <c r="J19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="1">
         <v>1</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M19" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>28</v>
@@ -1709,19 +1809,22 @@
         <v>28</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1752,35 +1855,38 @@
       <c r="J20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M20" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>49</v>
       </c>
@@ -1801,8 +1907,9 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>16</v>
       </c>
@@ -1833,35 +1940,38 @@
       <c r="J22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="1">
         <v>1</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -1892,14 +2002,14 @@
       <c r="J23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="1">
         <v>1</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M23" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>28</v>
@@ -1908,19 +2018,22 @@
         <v>28</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>18</v>
       </c>
@@ -1951,35 +2064,38 @@
       <c r="J24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="1">
         <v>1</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M24" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>19</v>
       </c>
@@ -2010,40 +2126,43 @@
       <c r="J25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="1">
         <v>1</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M25" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -2075,34 +2194,37 @@
         <v>16</v>
       </c>
       <c r="K27" s="1">
+        <v>120</v>
+      </c>
+      <c r="L27" s="1">
         <v>2</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P27" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -2134,34 +2256,37 @@
         <v>16</v>
       </c>
       <c r="K28" s="1">
+        <v>120</v>
+      </c>
+      <c r="L28" s="1">
         <v>2</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P28" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -2193,13 +2318,13 @@
         <v>16</v>
       </c>
       <c r="K29" s="1">
+        <v>120</v>
+      </c>
+      <c r="L29" s="1">
         <v>2</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M29" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>28</v>
@@ -2208,19 +2333,22 @@
         <v>28</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -2251,35 +2379,38 @@
       <c r="J30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="1">
         <v>2</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>24</v>
       </c>
@@ -2310,14 +2441,14 @@
       <c r="J31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" s="1">
         <v>2</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M31" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>28</v>
@@ -2326,19 +2457,22 @@
         <v>28</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>25</v>
       </c>
@@ -2369,35 +2503,38 @@
       <c r="J32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" s="1">
         <v>2</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M32" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>51</v>
       </c>
@@ -2418,8 +2555,9 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -2450,35 +2588,38 @@
       <c r="J34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" s="1">
         <v>2</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P34" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -2509,14 +2650,14 @@
       <c r="J35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="1">
         <v>2</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M35" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>28</v>
@@ -2525,19 +2666,22 @@
         <v>28</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -2568,35 +2712,38 @@
       <c r="J36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" s="1">
         <v>2</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M36" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P36" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -2627,35 +2774,38 @@
       <c r="J37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="1">
         <v>2</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M37" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P37" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>52</v>
       </c>
@@ -2676,8 +2826,9 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T38" s="1"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -2709,34 +2860,37 @@
         <v>16</v>
       </c>
       <c r="K39" s="1">
+        <v>120</v>
+      </c>
+      <c r="L39" s="1">
         <v>0</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P39" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>31</v>
       </c>
@@ -2768,34 +2922,37 @@
         <v>16</v>
       </c>
       <c r="K40" s="1">
+        <v>120</v>
+      </c>
+      <c r="L40" s="1">
         <v>0</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P40" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -2827,13 +2984,13 @@
         <v>16</v>
       </c>
       <c r="K41" s="1">
+        <v>120</v>
+      </c>
+      <c r="L41" s="1">
         <v>0</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M41" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>28</v>
@@ -2842,19 +2999,22 @@
         <v>28</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>33</v>
       </c>
@@ -2885,35 +3045,38 @@
       <c r="J42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L42" s="1">
         <v>0</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P42" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>34</v>
       </c>
@@ -2944,14 +3107,14 @@
       <c r="J43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L43" s="1">
         <v>0</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M43" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>28</v>
@@ -2960,19 +3123,22 @@
         <v>28</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>35</v>
       </c>
@@ -3003,35 +3169,38 @@
       <c r="J44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L44" s="1">
         <v>0</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M44" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P44" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>53</v>
       </c>
@@ -3052,8 +3221,9 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>36</v>
       </c>
@@ -3084,35 +3254,38 @@
       <c r="J46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L46" s="1">
         <v>0</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P46" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>37</v>
       </c>
@@ -3143,14 +3316,14 @@
       <c r="J47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L47" s="1">
         <v>0</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M47" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>28</v>
@@ -3159,19 +3332,22 @@
         <v>28</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>38</v>
       </c>
@@ -3202,35 +3378,38 @@
       <c r="J48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L48" s="1">
         <v>0</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M48" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P48" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q48" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>39</v>
       </c>
@@ -3261,35 +3440,38 @@
       <c r="J49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L49" s="1">
         <v>0</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M49" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O49" s="1" t="s">
+      <c r="P49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P49" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q49" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>54</v>
       </c>
@@ -3310,8 +3492,9 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T50" s="1"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>40</v>
       </c>
@@ -3343,34 +3526,37 @@
         <v>16</v>
       </c>
       <c r="K51" s="1">
+        <v>120</v>
+      </c>
+      <c r="L51" s="1">
         <v>1</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N51" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O51" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P51" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S51" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>41</v>
       </c>
@@ -3402,34 +3588,37 @@
         <v>16</v>
       </c>
       <c r="K52" s="1">
+        <v>120</v>
+      </c>
+      <c r="L52" s="1">
         <v>1</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P52" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="T52" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>42</v>
       </c>
@@ -3461,13 +3650,13 @@
         <v>16</v>
       </c>
       <c r="K53" s="1">
+        <v>120</v>
+      </c>
+      <c r="L53" s="1">
         <v>1</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M53" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>28</v>
@@ -3476,19 +3665,22 @@
         <v>28</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S53" s="1" t="s">
+      <c r="T53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>43</v>
       </c>
@@ -3519,35 +3711,38 @@
       <c r="J54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L54" s="1">
         <v>1</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N54" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="1" t="s">
+      <c r="P54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="T54" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>44</v>
       </c>
@@ -3578,14 +3773,14 @@
       <c r="J55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" s="1">
         <v>1</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M55" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>28</v>
@@ -3594,19 +3789,22 @@
         <v>28</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S55" s="1" t="s">
+      <c r="T55" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>45</v>
       </c>
@@ -3637,35 +3835,38 @@
       <c r="J56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="1">
         <v>1</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M56" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O56" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O56" s="1" t="s">
+      <c r="P56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P56" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q56" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S56" s="1" t="s">
+      <c r="T56" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -3686,8 +3887,9 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T57" s="1"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>46</v>
       </c>
@@ -3718,35 +3920,38 @@
       <c r="J58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L58" s="1">
         <v>1</v>
       </c>
-      <c r="L58" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N58" s="1" t="s">
+      <c r="O58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O58" s="1" t="s">
+      <c r="P58" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P58" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S58" s="1" t="s">
+      <c r="T58" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>47</v>
       </c>
@@ -3777,14 +3982,14 @@
       <c r="J59" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L59" s="1">
         <v>1</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M59" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>28</v>
@@ -3793,19 +3998,22 @@
         <v>28</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S59" s="1" t="s">
+      <c r="T59" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>48</v>
       </c>
@@ -3836,35 +4044,38 @@
       <c r="J60" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L60" s="1">
         <v>1</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M60" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O60" s="1" t="s">
+      <c r="P60" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P60" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q60" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S60" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S60" s="1" t="s">
+      <c r="T60" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>49</v>
       </c>
@@ -3895,35 +4106,38 @@
       <c r="J61" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L61" s="1">
         <v>1</v>
       </c>
-      <c r="L61" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M61" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O61" s="1" t="s">
+      <c r="P61" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P61" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S61" s="1" t="s">
+      <c r="T61" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>56</v>
       </c>
@@ -3944,8 +4158,9 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T62" s="1"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>50</v>
       </c>
@@ -3977,34 +4192,37 @@
         <v>16</v>
       </c>
       <c r="K63" s="1">
+        <v>120</v>
+      </c>
+      <c r="L63" s="1">
         <v>2</v>
       </c>
-      <c r="L63" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N63" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O63" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P63" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q63" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S63" s="1" t="s">
+      <c r="T63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>51</v>
       </c>
@@ -4036,34 +4254,37 @@
         <v>16</v>
       </c>
       <c r="K64" s="1">
+        <v>120</v>
+      </c>
+      <c r="L64" s="1">
         <v>2</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N64" s="1" t="s">
+      <c r="O64" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O64" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P64" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q64" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S64" s="1" t="s">
+      <c r="T64" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>52</v>
       </c>
@@ -4095,13 +4316,13 @@
         <v>16</v>
       </c>
       <c r="K65" s="1">
+        <v>120</v>
+      </c>
+      <c r="L65" s="1">
         <v>2</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M65" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>28</v>
@@ -4110,19 +4331,22 @@
         <v>28</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S65" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S65" s="1" t="s">
+      <c r="T65" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>53</v>
       </c>
@@ -4153,35 +4377,38 @@
       <c r="J66" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" s="1">
         <v>2</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N66" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N66" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O66" s="1" t="s">
+      <c r="P66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P66" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q66" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S66" s="1" t="s">
+      <c r="T66" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>54</v>
       </c>
@@ -4212,14 +4439,14 @@
       <c r="J67" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K67" s="1">
+      <c r="K67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L67" s="1">
         <v>2</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M67" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>28</v>
@@ -4228,19 +4455,22 @@
         <v>28</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S67" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S67" s="1" t="s">
+      <c r="T67" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>55</v>
       </c>
@@ -4271,35 +4501,38 @@
       <c r="J68" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="1">
         <v>2</v>
       </c>
-      <c r="L68" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M68" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O68" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O68" s="1" t="s">
+      <c r="P68" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P68" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q68" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S68" s="1" t="s">
+      <c r="T68" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>57</v>
       </c>
@@ -4320,8 +4553,9 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T69" s="1"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>56</v>
       </c>
@@ -4352,35 +4586,38 @@
       <c r="J70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K70" s="1">
+      <c r="K70" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L70" s="1">
         <v>2</v>
       </c>
-      <c r="L70" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N70" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N70" s="1" t="s">
+      <c r="O70" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O70" s="1" t="s">
+      <c r="P70" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P70" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q70" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S70" s="1" t="s">
+      <c r="T70" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>57</v>
       </c>
@@ -4411,14 +4648,14 @@
       <c r="J71" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K71" s="1">
+      <c r="K71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L71" s="1">
         <v>2</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M71" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>28</v>
@@ -4427,19 +4664,22 @@
         <v>28</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S71" s="1" t="s">
+      <c r="T71" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>58</v>
       </c>
@@ -4470,35 +4710,38 @@
       <c r="J72" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K72" s="1">
+      <c r="K72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L72" s="1">
         <v>2</v>
       </c>
-      <c r="L72" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M72" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O72" s="1" t="s">
+      <c r="P72" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P72" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q72" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S72" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S72" s="1" t="s">
+      <c r="T72" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>59</v>
       </c>
@@ -4529,31 +4772,34 @@
       <c r="J73" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K73" s="1">
+      <c r="K73" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L73" s="1">
         <v>2</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M73" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O73" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O73" s="1" t="s">
+      <c r="P73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P73" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q73" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S73" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S73" s="1" t="s">
+      <c r="T73" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>